<commit_message>
feat: everything except ncr
</commit_message>
<xml_diff>
--- a/data/NATIONAL CAPITAL REGION/TAGUIG - PATEROS.xlsx
+++ b/data/NATIONAL CAPITAL REGION/TAGUIG - PATEROS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D300"/>
+  <dimension ref="A1:D347"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5227,6 +5227,601 @@
         </is>
       </c>
     </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>MAYOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="inlineStr">
+        <is>
+          <t>Candidate</t>
+        </is>
+      </c>
+      <c r="B305" s="1" t="inlineStr">
+        <is>
+          <t>Votes</t>
+        </is>
+      </c>
+      <c r="C305" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>CAYETANO, ATE LANI (NP)</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>272,876</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>75.76 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>CERAFICA, ARNEL (PPP)</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>87,266</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>24.23 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="inlineStr">
+        <is>
+          <t>Over-votes</t>
+        </is>
+      </c>
+      <c r="B309" s="1" t="inlineStr">
+        <is>
+          <t>Under-votes</t>
+        </is>
+      </c>
+      <c r="C309" s="1" t="inlineStr">
+        <is>
+          <t>Valid votes</t>
+        </is>
+      </c>
+      <c r="D309" s="1" t="inlineStr">
+        <is>
+          <t>Votes obtained by all candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1183</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>9723</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>371575</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>360142</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>VICE-MAYOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="inlineStr">
+        <is>
+          <t>Candidate</t>
+        </is>
+      </c>
+      <c r="B315" s="1" t="inlineStr">
+        <is>
+          <t>Votes</t>
+        </is>
+      </c>
+      <c r="C315" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>ALIT, ARVIN (NP)</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>232,034</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>68.81 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>CERAFICA, JANELLE (PPP)</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>105,157</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>31.18 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="inlineStr">
+        <is>
+          <t>Over-votes</t>
+        </is>
+      </c>
+      <c r="B319" s="1" t="inlineStr">
+        <is>
+          <t>Under-votes</t>
+        </is>
+      </c>
+      <c r="C319" s="1" t="inlineStr">
+        <is>
+          <t>Valid votes</t>
+        </is>
+      </c>
+      <c r="D319" s="1" t="inlineStr">
+        <is>
+          <t>Votes obtained by all candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>384</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>33473</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>371575</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>337191</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>MEMBER, SANGGUNIANG PANLUNGSOD</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="inlineStr">
+        <is>
+          <t>Candidate</t>
+        </is>
+      </c>
+      <c r="B325" s="1" t="inlineStr">
+        <is>
+          <t>Votes</t>
+        </is>
+      </c>
+      <c r="C325" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>AMOROSO, INOCENTES (IND)</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>10,681</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>0.97 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>AQUINO, COMMISSIONER (NP)</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>85,159</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>7.77 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>BAUTISTA, JONJON (PPP)</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>33,826</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>3.08 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>BERNAL, RJ (PPP)</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>27,270</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>2.49 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>CRUZ, JANNAH (PPP)</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>38,925</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>3.55 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>DE MESA, GIGI VALENZUELA (NP)</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>105,617</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>9.64 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>DELOS SANTOS, WARREN (PPP)</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>35,586</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>3.25 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>DIONISIO, WARREN (PPP)</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>41,554</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>3.79 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>FRANCO, RONET (PPP)</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>35,560</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>3.24 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>ICAY, ANGGUS (PPP)</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>50,475</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>4.61 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>LABAMPA, JIMMY (NP)</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>105,771</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>9.66 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>LONTOC, PAUL (IND)</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>24,923</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>2.27 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>MADRID, ELVIRA (PPP)</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>24,620</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>2.24 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>MAÑOSCA, TOTONG (NP)</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>83,719</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>7.64 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>MARCELINO, TIKBOY (NP)</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>96,695</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>8.83 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>OGALINOLA, CARLITO (NP)</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>93,044</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>8.49 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>OSORIO, MAR NORBERT (IND)</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>12,696</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>1.15 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>PANGA-CRUZ, ATTYJOY (NP)</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>94,514</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>8.63 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>SAN PEDRO, GAMIE (NP)</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>94,111</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>8.59 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="inlineStr">
+        <is>
+          <t>Over-votes</t>
+        </is>
+      </c>
+      <c r="B346" s="1" t="inlineStr">
+        <is>
+          <t>Under-votes</t>
+        </is>
+      </c>
+      <c r="C346" s="1" t="inlineStr">
+        <is>
+          <t>Valid votes</t>
+        </is>
+      </c>
+      <c r="D346" s="1" t="inlineStr">
+        <is>
+          <t>Votes obtained by all candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2266</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>245486</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>1360352</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>1094746</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>